<commit_message>
update templates and html database guidance
</commit_message>
<xml_diff>
--- a/docs/templates/ccrcn_cores_template.xlsx
+++ b/docs/templates/ccrcn_cores_template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">column_name</t>
   </si>
@@ -21,16 +21,16 @@
     <t xml:space="preserve">definition</t>
   </si>
   <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
     <t xml:space="preserve">field_type</t>
   </si>
   <si>
     <t xml:space="preserve">unit</t>
   </si>
   <si>
-    <t xml:space="preserve">text_format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values</t>
+    <t xml:space="preserve">variable_codes</t>
   </si>
   <si>
     <t xml:space="preserve">study_id</t>
@@ -48,6 +48,9 @@
     <t xml:space="preserve">Site identification code unique to each study.</t>
   </si>
   <si>
+    <t xml:space="preserve">optional</t>
+  </si>
+  <si>
     <t xml:space="preserve">core_id</t>
   </si>
   <si>
@@ -63,9 +66,6 @@
     <t xml:space="preserve">numeric</t>
   </si>
   <si>
-    <t xml:space="preserve">nominalYear</t>
-  </si>
-  <si>
     <t xml:space="preserve">YYYY</t>
   </si>
   <si>
@@ -75,9 +75,6 @@
     <t xml:space="preserve">Numeric month of year of core collection.</t>
   </si>
   <si>
-    <t xml:space="preserve">nominalMonth</t>
-  </si>
-  <si>
     <t xml:space="preserve">MM</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t xml:space="preserve">Numeric day of month of core collection.</t>
   </si>
   <si>
-    <t xml:space="preserve">nominalDay</t>
-  </si>
-  <si>
     <t xml:space="preserve">DD</t>
   </si>
   <si>
@@ -120,6 +114,9 @@
     <t xml:space="preserve">Accuracy of latitude and longitude measurement, if determined and recorded.</t>
   </si>
   <si>
+    <t xml:space="preserve">encouraged</t>
+  </si>
+  <si>
     <t xml:space="preserve">meter</t>
   </si>
   <si>
@@ -147,15 +144,15 @@
     <t xml:space="preserve">Surface elevation of the core relative to defined datum.</t>
   </si>
   <si>
-    <t xml:space="preserve">meters</t>
-  </si>
-  <si>
     <t xml:space="preserve">elevation_datum</t>
   </si>
   <si>
     <t xml:space="preserve">The datum relative to which the core elevation was measured against (For a complete list of datum names and aliases please refer to the ISO Geodedic Registry_https://iso.registry.bespire.eu/register/geodetic/VerticalDatum).</t>
   </si>
   <si>
+    <t xml:space="preserve">conditional</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAVD88 = A gravity-based geodetic datum, North American Vertical Datum of 1988; MSL = A tidal datum, Mean Sea Level as measured against a local tide gauge; MTL = A tidal datum, Mean Tidal Level as measured against a local tide gauge; MHW = A tidal datum, Mean High Water as measured against a local tide gauge; MHHW = A tidal datum, Mean Higher High Water as measured against a local tide gauge; MHHWS = A tidal datum, Mean Higher High Water for Spring Tides as measured against a local tide gauge; MLW = A tidal datum, Mean Low Water as measured against a local tide gauge; MLLW = A tidal datum, Mean Lower Low Water as measured against a local tide gauge.; NHN = TBD.; NAP = TBD.</t>
   </si>
   <si>
@@ -310,39 +307,6 @@
   </si>
   <si>
     <t xml:space="preserve">dimensionless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format, units, or variable codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTK; handheld; other high resolution; other moderate resolution; other low resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAVD88; MSL; MTL; MHW; MHHW; MHHWS; MLW; MLLW; NHN; NAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTK; other high resolution; LiDAR; DEM; other low resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estuarine; brine; saline; brackish; fresh; mixoeuhaline; polyhaline; mesohaline; oligohaline; estuarine C-CAP; palustrine C-CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field observation; measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emergent; scrub shrub; forested; forested to shrub; forested to emergent; seagrass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mangrove; swamp; scrub/shrub; marsh; seagrass; algal mat; unvegetated; mudflat; upland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high; mid; low; levee; back</t>
-  </si>
-  <si>
-    <t xml:space="preserve">core depth limited by length of corer; core depth represents deposit depth; not specified</t>
   </si>
 </sst>
 </file>
@@ -732,9 +696,11 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -746,35 +712,39 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -792,450 +762,504 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
     <row r="35">
@@ -1275,213 +1299,141 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="8.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="7.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="7.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="4.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="5.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="3.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="10.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="8.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="9.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="17.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="15.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="14.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="9.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="18.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="16.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="15.71" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="14.71" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="15.71" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="14.71" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="16.71" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="17.71" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="16.71" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="7.71" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="16.71" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="17.71" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="16.71" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="16.71" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="24.71" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="27.71" hidden="0" customWidth="1"/>
+    <col min="31" max="31" width="15.71" hidden="0" customWidth="1"/>
+    <col min="32" max="32" width="19.71" hidden="0" customWidth="1"/>
+    <col min="33" max="33" width="12.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R2" t="s">
-        <v>100</v>
-      </c>
-      <c r="S2" t="s">
-        <v>104</v>
-      </c>
-      <c r="T2" t="s">
-        <v>105</v>
-      </c>
-      <c r="U2" t="s">
-        <v>100</v>
-      </c>
-      <c r="V2" t="s">
-        <v>106</v>
-      </c>
-      <c r="W2" t="s">
-        <v>105</v>
-      </c>
-      <c r="X2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG2" t="s">
         <v>95</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>